<commit_message>
first example edit and second example
</commit_message>
<xml_diff>
--- a/jxls-demo-2/src/main/resources/secondTemplate.xlsx
+++ b/jxls-demo-2/src/main/resources/secondTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lundegaard\JXLSdemo\jxls-demo-1\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lundegaard\JXLSdemo\jxls-demo-2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF81523-0881-4A9C-9142-A1DFD685F40D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA951F2-A6D0-43AC-8BFF-423282F0B7C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{F9F9C28E-AC2B-44DC-85F1-1BB10F8ED183}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <author>Jan Jaroš</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{307FD08B-F498-45AE-A30F-E1E2D4621A70}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{E8E5A26F-D304-40AE-BB9D-D166E6E51625}">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Jan Jaroš:</t>
         </r>
@@ -55,14 +55,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="F4")</t>
+jx:area(lastCell="C6")</t>
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{AFF016D7-DEAE-4E32-BF5A-BDBEDDB89290}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{629C6755-3A4A-47BC-825A-5799C906871A}">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Jan Jaroš:</t>
         </r>
@@ -79,10 +79,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="addresses" var="address" lastCell="F3")</t>
+jx:grid(lastCell="C5" headers="headers" data="data" areas=[C4:C4, C5:C5])</t>
         </r>
       </text>
     </comment>
@@ -91,37 +91,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Street</t>
+    <t>${header}</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>House number</t>
-  </si>
-  <si>
-    <t>ZIP Code</t>
-  </si>
-  <si>
-    <t>${address.city}</t>
-  </si>
-  <si>
-    <t>${address.zipCode}</t>
-  </si>
-  <si>
-    <t>${address.houseNumber}</t>
-  </si>
-  <si>
-    <t>${address.street}</t>
+    <t>${cell}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,21 +115,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -157,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,13 +141,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,17 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -514,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BD88B3-1A8F-451C-B939-B56A72082243}">
-  <dimension ref="B2:F4"/>
+  <dimension ref="C3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,42 +489,15 @@
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E4" s="3">
-        <f>SUM(E3)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <f>SUM(F3)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added email template and modified excel examples
</commit_message>
<xml_diff>
--- a/jxls-demo-2/src/main/resources/secondTemplate.xlsx
+++ b/jxls-demo-2/src/main/resources/secondTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lundegaard\JXLSdemo\jxls-demo-2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA951F2-A6D0-43AC-8BFF-423282F0B7C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B764E3E-A79C-4080-BCBE-4C3B9E9B30D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{F9F9C28E-AC2B-44DC-85F1-1BB10F8ED183}"/>
   </bookViews>
@@ -158,9 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -478,7 +483,7 @@
   <dimension ref="C3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +501,7 @@
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>